<commit_message>
tous les retours ont été corrigés
</commit_message>
<xml_diff>
--- a/graphique courbes.xlsx
+++ b/graphique courbes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\Joffrey\enjmin\algorithmique et programmation\TP note\tp-python-algo-tri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE3E8EE-9EED-4B19-B40E-00C8FE3F9879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA94111-7664-4D46-8CD2-A42A532E82A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generation de liste" sheetId="2" r:id="rId1"/>
@@ -1007,34 +1007,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.7726898193359299E-2</c:v>
+                  <c:v>2.8821706771850499E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.110095739364624</c:v>
+                  <c:v>0.16448330879211401</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21297407150268499</c:v>
+                  <c:v>0.36543011665344199</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.38732194900512601</c:v>
+                  <c:v>0.69101428985595703</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.61255979537963801</c:v>
+                  <c:v>1.01195263862609</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.932120561599731</c:v>
+                  <c:v>1.45066595077514</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2588913440704299</c:v>
+                  <c:v>2.0582830905914302</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.57381963729858</c:v>
+                  <c:v>2.85009288787841</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.00610303878784</c:v>
+                  <c:v>3.4401211738586399</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4676148891448899</c:v>
+                  <c:v>4.1274387836456299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6441,8 +6441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B1154C-DAAC-4837-8883-9C8BD276DC8D}">
   <dimension ref="C3:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -6451,8 +6451,8 @@
       <c r="C3">
         <v>1000</v>
       </c>
-      <c r="D3" s="4">
-        <v>1.7726898193359299E-2</v>
+      <c r="D3">
+        <v>2.8821706771850499E-2</v>
       </c>
     </row>
     <row r="4" spans="3:4">
@@ -6460,7 +6460,7 @@
         <v>2000</v>
       </c>
       <c r="D4" s="4">
-        <v>0.110095739364624</v>
+        <v>0.16448330879211401</v>
       </c>
     </row>
     <row r="5" spans="3:4">
@@ -6468,7 +6468,7 @@
         <v>3000</v>
       </c>
       <c r="D5" s="4">
-        <v>0.21297407150268499</v>
+        <v>0.36543011665344199</v>
       </c>
     </row>
     <row r="6" spans="3:4">
@@ -6476,7 +6476,7 @@
         <v>4000</v>
       </c>
       <c r="D6" s="4">
-        <v>0.38732194900512601</v>
+        <v>0.69101428985595703</v>
       </c>
     </row>
     <row r="7" spans="3:4">
@@ -6484,7 +6484,7 @@
         <v>5000</v>
       </c>
       <c r="D7" s="4">
-        <v>0.61255979537963801</v>
+        <v>1.01195263862609</v>
       </c>
     </row>
     <row r="8" spans="3:4">
@@ -6492,7 +6492,7 @@
         <v>6000</v>
       </c>
       <c r="D8" s="4">
-        <v>0.932120561599731</v>
+        <v>1.45066595077514</v>
       </c>
     </row>
     <row r="9" spans="3:4">
@@ -6500,7 +6500,7 @@
         <v>7000</v>
       </c>
       <c r="D9" s="4">
-        <v>1.2588913440704299</v>
+        <v>2.0582830905914302</v>
       </c>
     </row>
     <row r="10" spans="3:4">
@@ -6508,7 +6508,7 @@
         <v>8000</v>
       </c>
       <c r="D10" s="4">
-        <v>1.57381963729858</v>
+        <v>2.85009288787841</v>
       </c>
     </row>
     <row r="11" spans="3:4">
@@ -6516,7 +6516,7 @@
         <v>9000</v>
       </c>
       <c r="D11" s="4">
-        <v>2.00610303878784</v>
+        <v>3.4401211738586399</v>
       </c>
     </row>
     <row r="12" spans="3:4">
@@ -6524,7 +6524,7 @@
         <v>10000</v>
       </c>
       <c r="D12" s="4">
-        <v>2.4676148891448899</v>
+        <v>4.1274387836456299</v>
       </c>
     </row>
   </sheetData>
@@ -6729,7 +6729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30F36DF-0907-4515-80AC-DA0F35503E4D}">
   <dimension ref="B5:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>